<commit_message>
Started filling out Soviet divisonal level
</commit_message>
<xml_diff>
--- a/_reference/German OOBs.xlsx
+++ b/_reference/German OOBs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BRD Fallschirmjaeger" sheetId="25" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="43">
   <si>
     <t>TOTAL</t>
   </si>
@@ -37,6 +37,9 @@
     <t>Personnel ea</t>
   </si>
   <si>
+    <t>Truck</t>
+  </si>
+  <si>
     <t>MILAN</t>
   </si>
   <si>
@@ -94,9 +97,6 @@
     <t>MG3</t>
   </si>
   <si>
-    <t>BRD Panzer Brigade</t>
-  </si>
-  <si>
     <t>HQ</t>
   </si>
   <si>
@@ -106,9 +106,6 @@
     <t>PzGr Btn</t>
   </si>
   <si>
-    <t>(war btn?)</t>
-  </si>
-  <si>
     <t>Artillery</t>
   </si>
   <si>
@@ -121,28 +118,43 @@
     <t>Marder</t>
   </si>
   <si>
-    <t>120mm Mortar</t>
-  </si>
-  <si>
-    <t>152 SPH</t>
-  </si>
-  <si>
-    <t>TOW Jaguar</t>
-  </si>
-  <si>
     <t>BRD Panzergrenadier Brigade</t>
   </si>
   <si>
-    <t>Luchs</t>
-  </si>
-  <si>
     <t>MG-3</t>
   </si>
   <si>
     <t>PzF-44</t>
   </si>
   <si>
-    <t>12*3</t>
+    <t>BRD Panzerbrigade</t>
+  </si>
+  <si>
+    <t>G3-SG1</t>
+  </si>
+  <si>
+    <t>M113A2</t>
+  </si>
+  <si>
+    <t>M109G</t>
+  </si>
+  <si>
+    <t>Jaguar 2</t>
+  </si>
+  <si>
+    <t>SpPz Luchs</t>
+  </si>
+  <si>
+    <t>Note 380 Leopard II tanks were produced between 1979 and 1982</t>
+  </si>
+  <si>
+    <t>This is 3 brigades of tanks</t>
+  </si>
+  <si>
+    <t>Mixed btn</t>
+  </si>
+  <si>
+    <t>M113 M252</t>
   </si>
 </sst>
 </file>
@@ -554,31 +566,31 @@
         <v>0</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J1" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T1" s="2"/>
       <c r="U1" s="6" t="s">
@@ -588,19 +600,19 @@
         <v>0</v>
       </c>
       <c r="W1" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="X1" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Y1" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z1" s="8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AA1" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AB1" s="8"/>
       <c r="AC1" s="9"/>
@@ -687,7 +699,7 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="5">
         <v>1</v>
@@ -726,7 +738,7 @@
         <v>98</v>
       </c>
       <c r="T3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="U3" s="5">
         <v>1</v>
@@ -755,7 +767,7 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B4" s="5">
         <v>4</v>
@@ -780,7 +792,7 @@
         <v>30</v>
       </c>
       <c r="T4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U4" s="5">
         <v>4</v>
@@ -805,7 +817,7 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="5">
         <v>3</v>
@@ -828,7 +840,7 @@
         <v>18</v>
       </c>
       <c r="T5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="U5" s="5">
         <v>3</v>
@@ -853,7 +865,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5">
         <v>2</v>
@@ -872,7 +884,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="T6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U6" s="5">
         <v>2</v>
@@ -897,7 +909,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -920,7 +932,7 @@
         <v>60</v>
       </c>
       <c r="T7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="U7" s="5">
         <v>1</v>
@@ -943,7 +955,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -971,7 +983,7 @@
         <v>30</v>
       </c>
       <c r="T8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U8" s="5">
         <v>1</v>
@@ -996,7 +1008,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5">
         <v>4</v>
@@ -1015,7 +1027,7 @@
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="T9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="U9" s="5">
         <v>4</v>
@@ -1040,7 +1052,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -1062,7 +1074,7 @@
         <v>8</v>
       </c>
       <c r="T10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="U10" s="5">
         <v>1</v>
@@ -1087,7 +1099,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -1109,7 +1121,7 @@
         <v>24</v>
       </c>
       <c r="T11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U11" s="5">
         <v>1</v>
@@ -1136,7 +1148,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
@@ -1158,7 +1170,7 @@
         <v>24</v>
       </c>
       <c r="T12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="U12" s="5">
         <v>1</v>
@@ -1310,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1327,9 +1339,9 @@
     <col min="11" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
@@ -1350,77 +1362,77 @@
         <v>25</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="L1" s="9"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="4">
         <f>SUM(D2:O2)</f>
-        <v>1080</v>
+        <v>1346</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:L2" si="0">SUMPRODUCT(D3:D54,$B$3:$B$54)</f>
-        <v>0</v>
+        <f>SUMPRODUCT(D3:D56,$B$3:$B$56)</f>
+        <v>164</v>
       </c>
       <c r="E2" s="3">
-        <f t="shared" si="0"/>
-        <v>164</v>
+        <f>SUMPRODUCT(E3:E56,$B$3:$B$56)</f>
+        <v>188</v>
       </c>
       <c r="F2" s="3">
-        <f t="shared" si="0"/>
-        <v>164</v>
+        <f>SUMPRODUCT(F3:F56,$B$3:$B$56)</f>
+        <v>188</v>
       </c>
       <c r="G2" s="3">
-        <f t="shared" si="0"/>
-        <v>435</v>
+        <f>SUMPRODUCT(G3:G56,$B$3:$B$56)</f>
+        <v>429</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" si="0"/>
-        <v>155</v>
+        <f>SUMPRODUCT(H3:H56,$B$3:$B$56)</f>
+        <v>167</v>
       </c>
       <c r="I2" s="3">
-        <f t="shared" si="0"/>
-        <v>90</v>
+        <f>SUMPRODUCT(I3:I56,$B$3:$B$56)</f>
+        <v>126</v>
       </c>
       <c r="J2" s="3">
-        <f t="shared" si="0"/>
+        <f>SUMPRODUCT(J3:J56,$B$3:$B$56)</f>
         <v>36</v>
       </c>
       <c r="K2" s="3">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="L2" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+        <f>SUMPRODUCT(K3:K56,$B$3:$B$56)</f>
+        <v>48</v>
+      </c>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
       </c>
       <c r="C3" s="4">
-        <f t="shared" ref="C3:C12" si="1">SUM(D3:O3)</f>
-        <v>108</v>
-      </c>
-      <c r="D3" s="3"/>
+        <f t="shared" ref="C3:C15" si="0">SUM(D3:O3)</f>
+        <v>110</v>
+      </c>
+      <c r="D3" s="3">
+        <v>2</v>
+      </c>
       <c r="E3" s="10">
         <v>41</v>
       </c>
@@ -1436,18 +1448,20 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" s="4">
-        <f t="shared" si="1"/>
-        <v>44</v>
-      </c>
-      <c r="D4" s="3"/>
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="3">
@@ -1457,96 +1471,95 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="4">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="3">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3">
+        <f>11+4</f>
+        <v>15</v>
+      </c>
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="5">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
-        <f>SUM(D6:O6)</f>
-        <v>6</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="4">
-        <f t="shared" si="1"/>
+        <f>SUM(D7:O7)</f>
+        <v>6</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3">
+        <v>6</v>
+      </c>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="5">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4">
+        <f t="shared" si="0"/>
         <v>18</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="5">
-        <v>3</v>
-      </c>
-      <c r="C8" s="4">
-        <f t="shared" si="1"/>
-        <v>12</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
       </c>
       <c r="C9" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="D9" s="3"/>
@@ -1554,66 +1567,146 @@
       <c r="F9" s="10"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="K9">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I9" s="3"/>
+      <c r="J9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="B10" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C10" s="4">
-        <f t="shared" si="1"/>
-        <v>216</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
       <c r="D10" s="3"/>
-      <c r="G10" s="3">
-        <f>6*4*3*3</f>
-        <v>216</v>
-      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="1"/>
-        <v>36</v>
+        <f t="shared" si="0"/>
+        <v>135</v>
       </c>
       <c r="D11" s="3"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
       <c r="G11" s="3">
-        <f>4*3*3</f>
-        <v>36</v>
+        <f>5*3*3*3</f>
+        <v>135</v>
       </c>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
-      <c r="G12" s="3" t="s">
-        <v>38</v>
+      <c r="G12" s="3">
+        <v>27</v>
       </c>
       <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="3">
+        <v>27</v>
+      </c>
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="4">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="3">
+        <f>27</f>
+        <v>27</v>
+      </c>
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" si="0"/>
+        <v>282</v>
+      </c>
+      <c r="D15">
+        <v>150</v>
+      </c>
+      <c r="E15">
+        <v>24</v>
+      </c>
+      <c r="F15">
+        <v>24</v>
+      </c>
+      <c r="G15">
+        <v>36</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1622,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1633,15 +1726,16 @@
     <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>2</v>
@@ -1662,16 +1756,16 @@
         <v>25</v>
       </c>
       <c r="H1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="I1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="9" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>28</v>
       </c>
       <c r="L1" s="9"/>
     </row>
@@ -1682,31 +1776,31 @@
       <c r="B2" s="5"/>
       <c r="C2" s="4">
         <f>SUM(D2:O2)</f>
-        <v>847</v>
+        <v>1583</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:L2" si="0">SUMPRODUCT(D3:D54,$B$3:$B$54)</f>
-        <v>0</v>
+        <v>160</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" si="0"/>
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>429</v>
       </c>
       <c r="G2" s="3">
         <f t="shared" si="0"/>
-        <v>183</v>
+        <v>429</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" si="0"/>
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="I2" s="3">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="J2" s="3">
         <f t="shared" si="0"/>
@@ -1714,7 +1808,7 @@
       </c>
       <c r="K2" s="3">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="L2" s="3">
         <f t="shared" si="0"/>
@@ -1723,7 +1817,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B3" s="5">
         <v>4</v>
@@ -1748,16 +1842,18 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B4" s="5">
         <v>3</v>
       </c>
       <c r="C4" s="4">
         <f t="shared" si="1"/>
-        <v>77</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>79</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2</v>
+      </c>
       <c r="E4" s="10"/>
       <c r="F4" s="3">
         <v>33</v>
@@ -1771,92 +1867,94 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>35</v>
       </c>
       <c r="B5" s="5">
         <v>2</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" si="1"/>
-        <v>63</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
       <c r="E5" s="10"/>
       <c r="F5" s="3">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="G5" s="3">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3">
-        <v>9</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>4</v>
       </c>
       <c r="B6" s="5">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C6" s="4">
         <f>SUM(D6:O6)</f>
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G6" s="3">
-        <v>6</v>
-      </c>
-      <c r="H6" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="H6" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B7" s="5">
         <v>5</v>
       </c>
       <c r="C7" s="4">
         <f t="shared" si="1"/>
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="10"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="F7" s="3">
+        <v>6</v>
+      </c>
+      <c r="G7" s="3">
+        <v>6</v>
+      </c>
       <c r="H7" s="3"/>
-      <c r="I7">
-        <v>18</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B8" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" s="4">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="10"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8">
-        <v>12</v>
+      <c r="I8" s="3">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B9" s="5">
         <v>3</v>
@@ -1870,44 +1968,124 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="K9">
+      <c r="J9">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="5">
+        <v>4</v>
+      </c>
       <c r="C10" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
+      <c r="K10">
+        <v>12</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
       <c r="C11" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>270</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="10"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="F11" s="3">
+        <v>135</v>
+      </c>
+      <c r="G11" s="3">
+        <v>135</v>
+      </c>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
       <c r="C12" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="10"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
+      <c r="F12" s="3">
+        <v>27</v>
+      </c>
+      <c r="G12" s="3">
+        <v>27</v>
+      </c>
       <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>27</v>
+      </c>
+      <c r="G13">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>27</v>
+      </c>
+      <c r="G14">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>150</v>
+      </c>
+      <c r="E15">
+        <v>24</v>
+      </c>
+      <c r="F15">
+        <v>36</v>
+      </c>
+      <c r="G15">
+        <v>36</v>
+      </c>
+      <c r="H15">
+        <v>12</v>
+      </c>
+      <c r="I15">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>